<commit_message>
imporove the chatbot performace
</commit_message>
<xml_diff>
--- a/fashion_orders.xlsx
+++ b/fashion_orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -597,37 +597,85 @@
           <t>Steven</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" t="n">
+        <v>508988751</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Sweater</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>XXL</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>4</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Abu dhabi</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ORD-20250301000448</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-03-01 00:04:48</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Steven</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>0508988751</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Sweater</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>XXL</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Brown</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Abu dhabi</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Jeans</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
         <is>
           <t>New</t>
         </is>

</xml_diff>

<commit_message>
imporove the chatbot performace and add indonisian
</commit_message>
<xml_diff>
--- a/fashion_orders.xlsx
+++ b/fashion_orders.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,11 @@
           <t>status</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>language</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -532,6 +537,7 @@
           <t>New</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -580,6 +586,7 @@
           <t>New</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -628,6 +635,7 @@
           <t>New</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -645,39 +653,248 @@
           <t>Steven</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" t="n">
+        <v>508988751</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Jeans</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>5</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Dubai</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ORD-20250301071419</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-03-01 07:14:19</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Steven</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>508988751</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Jeans</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Green</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>5</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Abu Dhabi</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ORD-20250301073023</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-03-01 07:30:23</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Can i see the product</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>My name is fee sidabalok</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>I want to order dress</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Jalan aries utama no.57 rt.3/rw.3 Meruya utara kembangan jakarta barat</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ORD-20250301172534</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-03-01 17:25:34</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Steven</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>0508988751</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Rok</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Ungu</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>5</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Abu dhabi</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ORD-20250301172706</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-03-01 17:27:06</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Steven</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0508988751</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>Jeans</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>S</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Green</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>XXL</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Dubai</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Abu Dhabi</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
         <is>
           <t>New</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>en</t>
         </is>
       </c>
     </row>

</xml_diff>